<commit_message>
typo in taxonomy updated
</commit_message>
<xml_diff>
--- a/taxonomy/taxonomy_tree.xlsx
+++ b/taxonomy/taxonomy_tree.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharonklinkenberg/GitHub/Statistics_Taxonomy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sharonklinkenberg/GitHub/ShareStats_website/taxonomy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A002DAF0-A003-6D41-8A25-000B53E5D651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1466AC37-FBB2-6343-BBFD-015E57AE3B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="15980" xr2:uid="{6E62A4E4-07FD-0D42-8783-702D06A05F59}"/>
   </bookViews>
@@ -734,9 +734,6 @@
     <t>Factor analysis/Explained variance</t>
   </si>
   <si>
-    <t>Factor analysis/Compontent correlation matrix</t>
-  </si>
-  <si>
     <t>Factor analysis/Scree plot</t>
   </si>
   <si>
@@ -1448,9 +1445,6 @@
     <t>Explained variance</t>
   </si>
   <si>
-    <t>Compontent correlation matrix</t>
-  </si>
-  <si>
     <t>Scree plot</t>
   </si>
   <si>
@@ -1497,6 +1491,12 @@
   </si>
   <si>
     <t>name_en</t>
+  </si>
+  <si>
+    <t>Factor analysis/component correlation matrix</t>
+  </si>
+  <si>
+    <t>component correlation matrix</t>
   </si>
 </sst>
 </file>
@@ -1552,9 +1552,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1592,7 +1592,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1698,7 +1698,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1840,7 +1840,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1850,8 +1850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{795CCFFB-2EEB-A641-95A2-CC193EB07979}">
   <dimension ref="A1:D251"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="185" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A227" zoomScale="185" workbookViewId="0">
+      <selection activeCell="D235" sqref="D235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1862,16 +1862,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" t="s">
         <v>250</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>251</v>
       </c>
-      <c r="C1" t="s">
-        <v>252</v>
-      </c>
       <c r="D1" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1879,10 +1879,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1910,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1924,7 +1924,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1938,7 +1938,7 @@
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1952,7 +1952,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1980,7 +1980,7 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1994,7 +1994,7 @@
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2022,7 +2022,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2036,7 +2036,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2050,7 +2050,7 @@
         <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2064,7 +2064,7 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2078,7 +2078,7 @@
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2092,7 +2092,7 @@
         <v>14</v>
       </c>
       <c r="D17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2106,7 +2106,7 @@
         <v>15</v>
       </c>
       <c r="D18" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2120,7 +2120,7 @@
         <v>16</v>
       </c>
       <c r="D19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2134,7 +2134,7 @@
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2148,7 +2148,7 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2162,7 +2162,7 @@
         <v>19</v>
       </c>
       <c r="D22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2176,7 +2176,7 @@
         <v>20</v>
       </c>
       <c r="D23" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2190,7 +2190,7 @@
         <v>21</v>
       </c>
       <c r="D24" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2204,7 +2204,7 @@
         <v>22</v>
       </c>
       <c r="D25" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2218,7 +2218,7 @@
         <v>23</v>
       </c>
       <c r="D26" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2232,7 +2232,7 @@
         <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -2246,7 +2246,7 @@
         <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -2260,7 +2260,7 @@
         <v>26</v>
       </c>
       <c r="D29" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2274,7 +2274,7 @@
         <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -2288,7 +2288,7 @@
         <v>28</v>
       </c>
       <c r="D31" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -2302,7 +2302,7 @@
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -2316,7 +2316,7 @@
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -2330,7 +2330,7 @@
         <v>31</v>
       </c>
       <c r="D34" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -2344,7 +2344,7 @@
         <v>32</v>
       </c>
       <c r="D35" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -2358,7 +2358,7 @@
         <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -2372,7 +2372,7 @@
         <v>34</v>
       </c>
       <c r="D37" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -2386,7 +2386,7 @@
         <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -2400,7 +2400,7 @@
         <v>36</v>
       </c>
       <c r="D39" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -2414,7 +2414,7 @@
         <v>37</v>
       </c>
       <c r="D40" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -2428,7 +2428,7 @@
         <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -2442,7 +2442,7 @@
         <v>39</v>
       </c>
       <c r="D42" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -2456,7 +2456,7 @@
         <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -2484,7 +2484,7 @@
         <v>42</v>
       </c>
       <c r="D45" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -2498,7 +2498,7 @@
         <v>43</v>
       </c>
       <c r="D46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -2512,7 +2512,7 @@
         <v>44</v>
       </c>
       <c r="D47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -2526,7 +2526,7 @@
         <v>45</v>
       </c>
       <c r="D48" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -2540,7 +2540,7 @@
         <v>46</v>
       </c>
       <c r="D49" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -2554,7 +2554,7 @@
         <v>47</v>
       </c>
       <c r="D50" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -2568,7 +2568,7 @@
         <v>48</v>
       </c>
       <c r="D51" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -2582,7 +2582,7 @@
         <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -2596,7 +2596,7 @@
         <v>50</v>
       </c>
       <c r="D53" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -2610,7 +2610,7 @@
         <v>51</v>
       </c>
       <c r="D54" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -2624,7 +2624,7 @@
         <v>52</v>
       </c>
       <c r="D55" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2638,7 +2638,7 @@
         <v>53</v>
       </c>
       <c r="D56" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -2652,7 +2652,7 @@
         <v>54</v>
       </c>
       <c r="D57" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -2666,7 +2666,7 @@
         <v>55</v>
       </c>
       <c r="D58" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -2680,7 +2680,7 @@
         <v>56</v>
       </c>
       <c r="D59" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -2694,7 +2694,7 @@
         <v>57</v>
       </c>
       <c r="D60" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -2708,7 +2708,7 @@
         <v>58</v>
       </c>
       <c r="D61" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -2722,7 +2722,7 @@
         <v>59</v>
       </c>
       <c r="D62" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -2736,7 +2736,7 @@
         <v>60</v>
       </c>
       <c r="D63" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -2750,7 +2750,7 @@
         <v>61</v>
       </c>
       <c r="D64" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -2764,7 +2764,7 @@
         <v>62</v>
       </c>
       <c r="D65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -2778,7 +2778,7 @@
         <v>63</v>
       </c>
       <c r="D66" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -2792,7 +2792,7 @@
         <v>64</v>
       </c>
       <c r="D67" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -2806,7 +2806,7 @@
         <v>65</v>
       </c>
       <c r="D68" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -2820,7 +2820,7 @@
         <v>66</v>
       </c>
       <c r="D69" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -2834,7 +2834,7 @@
         <v>67</v>
       </c>
       <c r="D70" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -2848,7 +2848,7 @@
         <v>68</v>
       </c>
       <c r="D71" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -2862,7 +2862,7 @@
         <v>69</v>
       </c>
       <c r="D72" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -2876,7 +2876,7 @@
         <v>70</v>
       </c>
       <c r="D73" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -2890,7 +2890,7 @@
         <v>71</v>
       </c>
       <c r="D74" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2904,7 +2904,7 @@
         <v>72</v>
       </c>
       <c r="D75" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2918,7 +2918,7 @@
         <v>73</v>
       </c>
       <c r="D76" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2932,7 +2932,7 @@
         <v>74</v>
       </c>
       <c r="D77" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2946,7 +2946,7 @@
         <v>75</v>
       </c>
       <c r="D78" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2960,7 +2960,7 @@
         <v>76</v>
       </c>
       <c r="D79" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2974,7 +2974,7 @@
         <v>77</v>
       </c>
       <c r="D80" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2988,7 +2988,7 @@
         <v>78</v>
       </c>
       <c r="D81" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -3002,7 +3002,7 @@
         <v>79</v>
       </c>
       <c r="D82" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -3016,7 +3016,7 @@
         <v>80</v>
       </c>
       <c r="D83" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -3030,7 +3030,7 @@
         <v>81</v>
       </c>
       <c r="D84" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -3044,7 +3044,7 @@
         <v>82</v>
       </c>
       <c r="D85" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -3058,7 +3058,7 @@
         <v>83</v>
       </c>
       <c r="D86" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -3072,7 +3072,7 @@
         <v>84</v>
       </c>
       <c r="D87" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -3086,7 +3086,7 @@
         <v>85</v>
       </c>
       <c r="D88" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -3100,7 +3100,7 @@
         <v>86</v>
       </c>
       <c r="D89" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -3114,7 +3114,7 @@
         <v>87</v>
       </c>
       <c r="D90" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -3128,7 +3128,7 @@
         <v>88</v>
       </c>
       <c r="D91" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -3142,7 +3142,7 @@
         <v>89</v>
       </c>
       <c r="D92" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -3156,7 +3156,7 @@
         <v>90</v>
       </c>
       <c r="D93" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -3170,7 +3170,7 @@
         <v>91</v>
       </c>
       <c r="D94" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -3184,7 +3184,7 @@
         <v>92</v>
       </c>
       <c r="D95" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -3198,7 +3198,7 @@
         <v>93</v>
       </c>
       <c r="D96" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -3212,7 +3212,7 @@
         <v>94</v>
       </c>
       <c r="D97" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -3226,7 +3226,7 @@
         <v>95</v>
       </c>
       <c r="D98" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -3240,7 +3240,7 @@
         <v>96</v>
       </c>
       <c r="D99" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -3254,7 +3254,7 @@
         <v>97</v>
       </c>
       <c r="D100" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -3268,7 +3268,7 @@
         <v>98</v>
       </c>
       <c r="D101" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -3282,7 +3282,7 @@
         <v>99</v>
       </c>
       <c r="D102" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -3296,7 +3296,7 @@
         <v>100</v>
       </c>
       <c r="D103" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -3310,7 +3310,7 @@
         <v>101</v>
       </c>
       <c r="D104" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -3324,7 +3324,7 @@
         <v>102</v>
       </c>
       <c r="D105" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -3338,7 +3338,7 @@
         <v>103</v>
       </c>
       <c r="D106" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -3352,7 +3352,7 @@
         <v>104</v>
       </c>
       <c r="D107" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -3366,7 +3366,7 @@
         <v>105</v>
       </c>
       <c r="D108" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -3380,7 +3380,7 @@
         <v>106</v>
       </c>
       <c r="D109" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -3394,7 +3394,7 @@
         <v>107</v>
       </c>
       <c r="D110" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -3408,7 +3408,7 @@
         <v>108</v>
       </c>
       <c r="D111" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -3422,7 +3422,7 @@
         <v>109</v>
       </c>
       <c r="D112" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -3436,7 +3436,7 @@
         <v>110</v>
       </c>
       <c r="D113" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -3450,7 +3450,7 @@
         <v>111</v>
       </c>
       <c r="D114" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -3464,7 +3464,7 @@
         <v>112</v>
       </c>
       <c r="D115" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -3478,7 +3478,7 @@
         <v>113</v>
       </c>
       <c r="D116" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -3492,7 +3492,7 @@
         <v>114</v>
       </c>
       <c r="D117" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -3506,7 +3506,7 @@
         <v>115</v>
       </c>
       <c r="D118" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -3520,7 +3520,7 @@
         <v>116</v>
       </c>
       <c r="D119" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -3534,7 +3534,7 @@
         <v>117</v>
       </c>
       <c r="D120" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -3548,7 +3548,7 @@
         <v>118</v>
       </c>
       <c r="D121" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -3562,7 +3562,7 @@
         <v>119</v>
       </c>
       <c r="D122" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -3576,7 +3576,7 @@
         <v>120</v>
       </c>
       <c r="D123" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -3590,7 +3590,7 @@
         <v>121</v>
       </c>
       <c r="D124" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -3604,7 +3604,7 @@
         <v>122</v>
       </c>
       <c r="D125" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -3618,7 +3618,7 @@
         <v>123</v>
       </c>
       <c r="D126" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -3632,7 +3632,7 @@
         <v>124</v>
       </c>
       <c r="D127" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -3646,7 +3646,7 @@
         <v>125</v>
       </c>
       <c r="D128" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -3660,7 +3660,7 @@
         <v>126</v>
       </c>
       <c r="D129" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -3674,7 +3674,7 @@
         <v>127</v>
       </c>
       <c r="D130" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
@@ -3688,7 +3688,7 @@
         <v>128</v>
       </c>
       <c r="D131" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
@@ -3702,7 +3702,7 @@
         <v>129</v>
       </c>
       <c r="D132" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
@@ -3716,7 +3716,7 @@
         <v>130</v>
       </c>
       <c r="D133" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -3730,7 +3730,7 @@
         <v>131</v>
       </c>
       <c r="D134" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -3744,7 +3744,7 @@
         <v>132</v>
       </c>
       <c r="D135" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.2">
@@ -3758,7 +3758,7 @@
         <v>133</v>
       </c>
       <c r="D136" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.2">
@@ -3772,7 +3772,7 @@
         <v>134</v>
       </c>
       <c r="D137" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.2">
@@ -3786,7 +3786,7 @@
         <v>135</v>
       </c>
       <c r="D138" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.2">
@@ -3800,7 +3800,7 @@
         <v>136</v>
       </c>
       <c r="D139" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -3814,7 +3814,7 @@
         <v>137</v>
       </c>
       <c r="D140" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -3828,7 +3828,7 @@
         <v>138</v>
       </c>
       <c r="D141" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -3842,7 +3842,7 @@
         <v>139</v>
       </c>
       <c r="D142" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -3856,7 +3856,7 @@
         <v>140</v>
       </c>
       <c r="D143" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -3870,7 +3870,7 @@
         <v>141</v>
       </c>
       <c r="D144" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.2">
@@ -3884,7 +3884,7 @@
         <v>142</v>
       </c>
       <c r="D145" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.2">
@@ -3898,7 +3898,7 @@
         <v>143</v>
       </c>
       <c r="D146" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.2">
@@ -3912,7 +3912,7 @@
         <v>144</v>
       </c>
       <c r="D147" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.2">
@@ -3926,7 +3926,7 @@
         <v>145</v>
       </c>
       <c r="D148" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.2">
@@ -3940,7 +3940,7 @@
         <v>146</v>
       </c>
       <c r="D149" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.2">
@@ -3954,7 +3954,7 @@
         <v>147</v>
       </c>
       <c r="D150" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.2">
@@ -3968,7 +3968,7 @@
         <v>148</v>
       </c>
       <c r="D151" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.2">
@@ -3982,7 +3982,7 @@
         <v>149</v>
       </c>
       <c r="D152" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.2">
@@ -3996,7 +3996,7 @@
         <v>150</v>
       </c>
       <c r="D153" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.2">
@@ -4010,7 +4010,7 @@
         <v>151</v>
       </c>
       <c r="D154" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.2">
@@ -4024,7 +4024,7 @@
         <v>152</v>
       </c>
       <c r="D155" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
@@ -4038,7 +4038,7 @@
         <v>153</v>
       </c>
       <c r="D156" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.2">
@@ -4052,7 +4052,7 @@
         <v>154</v>
       </c>
       <c r="D157" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.2">
@@ -4066,7 +4066,7 @@
         <v>155</v>
       </c>
       <c r="D158" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.2">
@@ -4080,7 +4080,7 @@
         <v>156</v>
       </c>
       <c r="D159" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.2">
@@ -4094,7 +4094,7 @@
         <v>157</v>
       </c>
       <c r="D160" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -4108,7 +4108,7 @@
         <v>158</v>
       </c>
       <c r="D161" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -4122,7 +4122,7 @@
         <v>159</v>
       </c>
       <c r="D162" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -4136,7 +4136,7 @@
         <v>160</v>
       </c>
       <c r="D163" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -4150,7 +4150,7 @@
         <v>161</v>
       </c>
       <c r="D164" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -4164,7 +4164,7 @@
         <v>162</v>
       </c>
       <c r="D165" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -4178,7 +4178,7 @@
         <v>163</v>
       </c>
       <c r="D166" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -4192,7 +4192,7 @@
         <v>164</v>
       </c>
       <c r="D167" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -4206,7 +4206,7 @@
         <v>165</v>
       </c>
       <c r="D168" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.2">
@@ -4234,7 +4234,7 @@
         <v>167</v>
       </c>
       <c r="D170" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.2">
@@ -4248,7 +4248,7 @@
         <v>168</v>
       </c>
       <c r="D171" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.2">
@@ -4262,7 +4262,7 @@
         <v>169</v>
       </c>
       <c r="D172" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.2">
@@ -4276,7 +4276,7 @@
         <v>170</v>
       </c>
       <c r="D173" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.2">
@@ -4290,7 +4290,7 @@
         <v>171</v>
       </c>
       <c r="D174" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.2">
@@ -4304,7 +4304,7 @@
         <v>172</v>
       </c>
       <c r="D175" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.2">
@@ -4318,7 +4318,7 @@
         <v>173</v>
       </c>
       <c r="D176" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.2">
@@ -4332,7 +4332,7 @@
         <v>174</v>
       </c>
       <c r="D177" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.2">
@@ -4346,7 +4346,7 @@
         <v>175</v>
       </c>
       <c r="D178" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.2">
@@ -4360,7 +4360,7 @@
         <v>176</v>
       </c>
       <c r="D179" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.2">
@@ -4374,7 +4374,7 @@
         <v>177</v>
       </c>
       <c r="D180" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.2">
@@ -4388,7 +4388,7 @@
         <v>178</v>
       </c>
       <c r="D181" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.2">
@@ -4402,7 +4402,7 @@
         <v>179</v>
       </c>
       <c r="D182" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.2">
@@ -4416,7 +4416,7 @@
         <v>180</v>
       </c>
       <c r="D183" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.2">
@@ -4430,7 +4430,7 @@
         <v>181</v>
       </c>
       <c r="D184" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.2">
@@ -4444,7 +4444,7 @@
         <v>182</v>
       </c>
       <c r="D185" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.2">
@@ -4458,7 +4458,7 @@
         <v>183</v>
       </c>
       <c r="D186" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.2">
@@ -4486,7 +4486,7 @@
         <v>185</v>
       </c>
       <c r="D188" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.2">
@@ -4500,7 +4500,7 @@
         <v>186</v>
       </c>
       <c r="D189" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.2">
@@ -4514,7 +4514,7 @@
         <v>187</v>
       </c>
       <c r="D190" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
@@ -4528,7 +4528,7 @@
         <v>188</v>
       </c>
       <c r="D191" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
@@ -4542,7 +4542,7 @@
         <v>189</v>
       </c>
       <c r="D192" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
@@ -4556,7 +4556,7 @@
         <v>190</v>
       </c>
       <c r="D193" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
@@ -4570,7 +4570,7 @@
         <v>191</v>
       </c>
       <c r="D194" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
@@ -4584,7 +4584,7 @@
         <v>192</v>
       </c>
       <c r="D195" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
@@ -4598,7 +4598,7 @@
         <v>193</v>
       </c>
       <c r="D196" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
@@ -4612,7 +4612,7 @@
         <v>194</v>
       </c>
       <c r="D197" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
@@ -4626,7 +4626,7 @@
         <v>195</v>
       </c>
       <c r="D198" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
@@ -4640,7 +4640,7 @@
         <v>196</v>
       </c>
       <c r="D199" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
@@ -4654,7 +4654,7 @@
         <v>197</v>
       </c>
       <c r="D200" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
@@ -4668,7 +4668,7 @@
         <v>198</v>
       </c>
       <c r="D201" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
@@ -4682,7 +4682,7 @@
         <v>199</v>
       </c>
       <c r="D202" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
@@ -4696,7 +4696,7 @@
         <v>200</v>
       </c>
       <c r="D203" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
@@ -4710,7 +4710,7 @@
         <v>201</v>
       </c>
       <c r="D204" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
@@ -4724,7 +4724,7 @@
         <v>202</v>
       </c>
       <c r="D205" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
@@ -4738,7 +4738,7 @@
         <v>203</v>
       </c>
       <c r="D206" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
@@ -4752,7 +4752,7 @@
         <v>204</v>
       </c>
       <c r="D207" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
@@ -4766,7 +4766,7 @@
         <v>205</v>
       </c>
       <c r="D208" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
@@ -4794,7 +4794,7 @@
         <v>207</v>
       </c>
       <c r="D210" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
@@ -4808,7 +4808,7 @@
         <v>208</v>
       </c>
       <c r="D211" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
@@ -4822,7 +4822,7 @@
         <v>209</v>
       </c>
       <c r="D212" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
@@ -4836,7 +4836,7 @@
         <v>210</v>
       </c>
       <c r="D213" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
@@ -4850,7 +4850,7 @@
         <v>211</v>
       </c>
       <c r="D214" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
@@ -4864,7 +4864,7 @@
         <v>212</v>
       </c>
       <c r="D215" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
@@ -4878,7 +4878,7 @@
         <v>213</v>
       </c>
       <c r="D216" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
@@ -4892,7 +4892,7 @@
         <v>214</v>
       </c>
       <c r="D217" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
@@ -4906,7 +4906,7 @@
         <v>215</v>
       </c>
       <c r="D218" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
@@ -4920,7 +4920,7 @@
         <v>216</v>
       </c>
       <c r="D219" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
@@ -4934,7 +4934,7 @@
         <v>217</v>
       </c>
       <c r="D220" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
@@ -4948,7 +4948,7 @@
         <v>218</v>
       </c>
       <c r="D221" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
@@ -4962,7 +4962,7 @@
         <v>219</v>
       </c>
       <c r="D222" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
@@ -4976,7 +4976,7 @@
         <v>220</v>
       </c>
       <c r="D223" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -4990,7 +4990,7 @@
         <v>221</v>
       </c>
       <c r="D224" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
@@ -5004,7 +5004,7 @@
         <v>222</v>
       </c>
       <c r="D225" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
@@ -5018,7 +5018,7 @@
         <v>223</v>
       </c>
       <c r="D226" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
@@ -5046,7 +5046,7 @@
         <v>225</v>
       </c>
       <c r="D228" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
@@ -5060,7 +5060,7 @@
         <v>226</v>
       </c>
       <c r="D229" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
@@ -5074,7 +5074,7 @@
         <v>227</v>
       </c>
       <c r="D230" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
@@ -5088,7 +5088,7 @@
         <v>228</v>
       </c>
       <c r="D231" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
@@ -5102,7 +5102,7 @@
         <v>229</v>
       </c>
       <c r="D232" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
@@ -5116,7 +5116,7 @@
         <v>230</v>
       </c>
       <c r="D233" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
@@ -5130,7 +5130,7 @@
         <v>231</v>
       </c>
       <c r="D234" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
@@ -5141,10 +5141,10 @@
         <v>234</v>
       </c>
       <c r="C235" t="s">
-        <v>232</v>
+        <v>485</v>
       </c>
       <c r="D235" t="s">
-        <v>470</v>
+        <v>486</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
@@ -5155,10 +5155,10 @@
         <v>235</v>
       </c>
       <c r="C236" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D236" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
@@ -5169,10 +5169,10 @@
         <v>236</v>
       </c>
       <c r="C237" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D237" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
@@ -5183,10 +5183,10 @@
         <v>237</v>
       </c>
       <c r="C238" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D238" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
@@ -5197,10 +5197,10 @@
         <v>238</v>
       </c>
       <c r="C239" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D239" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
@@ -5211,10 +5211,10 @@
         <v>239</v>
       </c>
       <c r="C240" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D240" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
@@ -5225,10 +5225,10 @@
         <v>240</v>
       </c>
       <c r="C241" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D241" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
@@ -5239,10 +5239,10 @@
         <v>241</v>
       </c>
       <c r="C242" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D242" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
@@ -5253,10 +5253,10 @@
         <v>242</v>
       </c>
       <c r="C243" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D243" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
@@ -5267,10 +5267,10 @@
         <v>243</v>
       </c>
       <c r="C244" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D244" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
@@ -5281,10 +5281,10 @@
         <v>244</v>
       </c>
       <c r="C245" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D245" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
@@ -5295,10 +5295,10 @@
         <v>245</v>
       </c>
       <c r="C246" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D246" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
@@ -5309,10 +5309,10 @@
         <v>246</v>
       </c>
       <c r="C247" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D247" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
@@ -5323,10 +5323,10 @@
         <v>247</v>
       </c>
       <c r="C248" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D248" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
@@ -5337,10 +5337,10 @@
         <v>248</v>
       </c>
       <c r="C249" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D249" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
@@ -5351,10 +5351,10 @@
         <v>249</v>
       </c>
       <c r="C250" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D250" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
@@ -5365,10 +5365,10 @@
         <v>250</v>
       </c>
       <c r="C251" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D251" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>

</xml_diff>